<commit_message>
tsv initial format fix
</commit_message>
<xml_diff>
--- a/conf/crule_test.xlsx
+++ b/conf/crule_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="crule_test" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t xml:space="preserve">@fastcner</t>
   </si>
@@ -64,16 +64,13 @@
     <t xml:space="preserve">with\s+(visual) change</t>
   </si>
   <si>
-    <t xml:space="preserve">PSEUDO_HEARING</t>
+    <t xml:space="preserve">HEARING</t>
   </si>
   <si>
     <t xml:space="preserve">PSEUDO</t>
   </si>
   <si>
     <t xml:space="preserve">hearing) changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEARING</t>
   </si>
   <si>
     <t xml:space="preserve">he (pa)t</t>
@@ -264,16 +261,16 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.48469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="7.86734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="7.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,7 +328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
@@ -353,12 +350,12 @@
         <v>0.5</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.5</v>
@@ -369,24 +366,24 @@
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>15</v>
@@ -394,30 +391,30 @@
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>